<commit_message>
Adição de novos casos de teste
</commit_message>
<xml_diff>
--- a/Documentação/Testes/Casos de teste.xlsx
+++ b/Documentação/Testes/Casos de teste.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Gerenciador-de-partidas\Documentação\Testes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Gerenciador-de-partidas-MpsBr\Documentação\Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="945" yWindow="600" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Entrada</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>CE_Login</t>
+  </si>
+  <si>
+    <t>login = bobbmarcio</t>
   </si>
   <si>
     <r>
@@ -60,16 +66,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">null; </t>
+      <t>null</t>
     </r>
+  </si>
+  <si>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>senha = 12345678</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">senha = </t>
     </r>
     <r>
@@ -85,22 +92,53 @@
     </r>
   </si>
   <si>
-    <t>login = bobbmarcio; senha = admin123</t>
-  </si>
-  <si>
-    <t>CE_Login</t>
-  </si>
-  <si>
-    <t>Criar Login</t>
-  </si>
-  <si>
-    <t>CE_CriarLogin</t>
-  </si>
-  <si>
-    <t>login = augusto01; senha = 12345678A</t>
-  </si>
-  <si>
-    <t>login = augusto01; senha = 123</t>
+    <t>CE_Senha</t>
+  </si>
+  <si>
+    <t>Nome do campeonato</t>
+  </si>
+  <si>
+    <t>nome = Campeonato Brasileiro</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nome = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <t>CE_NomeCampeonato</t>
+  </si>
+  <si>
+    <t>Quantidade de times</t>
+  </si>
+  <si>
+    <t>quantidade = 3...</t>
+  </si>
+  <si>
+    <t>quantidade = ..., -2, -1, 0, 1, 2</t>
+  </si>
+  <si>
+    <t>CE_QuantidadeTimes</t>
+  </si>
+  <si>
+    <t>Nome do time</t>
+  </si>
+  <si>
+    <t>nome = Corinthinas</t>
+  </si>
+  <si>
+    <t>CE_NomeTime</t>
   </si>
 </sst>
 </file>
@@ -124,12 +162,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,10 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,31 +507,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -498,10 +543,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,13 +554,55 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>